<commit_message>
+ gitignore, Excel Summing
</commit_message>
<xml_diff>
--- a/ShikoSumming.xlsx
+++ b/ShikoSumming.xlsx
@@ -9,11 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="13095" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13095" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Output">Sheet1!$B$4</definedName>
+    <definedName name="S_0">Sheet1!$D$5</definedName>
+    <definedName name="S_1">Sheet1!$D$6</definedName>
+    <definedName name="S_2">Sheet1!$D$7</definedName>
+    <definedName name="S_3">Sheet1!$D$8</definedName>
+    <definedName name="S0">Sheet1!$D$5</definedName>
+    <definedName name="tm">Sheet1!$B$3</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -458,7 +467,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,15 +518,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="3">
-        <v>701</v>
+        <v>780</v>
       </c>
       <c r="C6">
         <f>MAX(B6-$B$2,0)</f>
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1">
-        <f>QUOTIENT(D5*($B$3-C6),$B$3)</f>
-        <v>299</v>
+        <f>QUOTIENT(D5*(tm-C6),tm)</f>
+        <v>220</v>
       </c>
       <c r="G6">
         <f>300*(300-100)/300</f>
@@ -529,15 +538,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C8" si="0">MAX(B7-$B$2,0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D7:D8" si="1">QUOTIENT(D6*($B$3-C7),$B$3)</f>
-        <v>299</v>
+        <f>QUOTIENT(D6*(tm-C7),tm)</f>
+        <v>146</v>
       </c>
       <c r="H7">
         <f>(300-200-1)*4/300</f>
@@ -556,8 +565,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>299</v>
+        <f>QUOTIENT(D7*(tm-C8),tm)</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>(tm-S_3-1)*Output</f>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -565,8 +580,8 @@
         <v>7</v>
       </c>
       <c r="B10" s="5">
-        <f>FLOOR(($B$3-D8-1)*$B$4/$B$3,1)+1</f>
-        <v>1</v>
+        <f>IF(B9&gt;=0,QUOTIENT(B9,tm)+1,0)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pill3 for Beriozka prepared
</commit_message>
<xml_diff>
--- a/ShikoSumming.xlsx
+++ b/ShikoSumming.xlsx
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -518,15 +518,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="3">
-        <v>780</v>
+        <v>901</v>
       </c>
       <c r="C6">
         <f>MAX(B6-$B$2,0)</f>
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1">
         <f>QUOTIENT(D5*(tm-C6),tm)</f>
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="G6">
         <f>300*(300-100)/300</f>
@@ -538,15 +538,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C8" si="0">MAX(B7-$B$2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <f>QUOTIENT(D6*(tm-C7),tm)</f>
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="H7">
         <f>(300-200-1)*4/300</f>
@@ -566,13 +566,13 @@
       </c>
       <c r="D8" s="1">
         <f>QUOTIENT(D7*(tm-C8),tm)</f>
-        <v>146</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>(tm-S_3-1)*Output</f>
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>